<commit_message>
Good start on log
</commit_message>
<xml_diff>
--- a/TrainingMaterial/TrainingLog.xlsx
+++ b/TrainingMaterial/TrainingLog.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\TrainingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83896E84-B8A1-4ADE-89BB-2DB5B8D60B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB82E2CC-C6B6-4D93-8CE4-A87EBEAA8AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CD82CDFE-F1ED-40B0-B6ED-832A13DC569B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CD82CDFE-F1ED-40B0-B6ED-832A13DC569B}"/>
   </bookViews>
   <sheets>
     <sheet name="Objectives" sheetId="1" r:id="rId1"/>
+    <sheet name="W1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'W1'!$A$4:$I$52</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'W1'!$A$1:$W$22</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="71">
   <si>
     <t>Metrics</t>
   </si>
@@ -90,13 +95,172 @@
   </si>
   <si>
     <t>I think one week per sheet is what I need.</t>
+  </si>
+  <si>
+    <t>Inc. Press</t>
+  </si>
+  <si>
+    <t>Flat Press</t>
+  </si>
+  <si>
+    <t>Fly</t>
+  </si>
+  <si>
+    <t>Tri Ext</t>
+  </si>
+  <si>
+    <t>Inc Tri Pull</t>
+  </si>
+  <si>
+    <t>Side Curl</t>
+  </si>
+  <si>
+    <t>Std. Curl</t>
+  </si>
+  <si>
+    <t>Push Up</t>
+  </si>
+  <si>
+    <t>Dec Push Up</t>
+  </si>
+  <si>
+    <t>Inc Push Up</t>
+  </si>
+  <si>
+    <t>Hammer Curl</t>
+  </si>
+  <si>
+    <t>Arm</t>
+  </si>
+  <si>
+    <t>Legs</t>
+  </si>
+  <si>
+    <t>Bulgarian</t>
+  </si>
+  <si>
+    <t>Squat</t>
+  </si>
+  <si>
+    <t>Walk</t>
+  </si>
+  <si>
+    <t>Band Curl</t>
+  </si>
+  <si>
+    <t>Glut Bridge</t>
+  </si>
+  <si>
+    <t>Glut</t>
+  </si>
+  <si>
+    <t>Lung</t>
+  </si>
+  <si>
+    <t>Kickback</t>
+  </si>
+  <si>
+    <t>Tri Kickback</t>
+  </si>
+  <si>
+    <t>Plyo</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Exercise</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>WS</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>RM</t>
+  </si>
+  <si>
+    <t>WM</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>RT</t>
+  </si>
+  <si>
+    <t>WT</t>
+  </si>
+  <si>
+    <t>RW</t>
+  </si>
+  <si>
+    <t>WW</t>
+  </si>
+  <si>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>WR</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>WF</t>
+  </si>
+  <si>
+    <t>SU</t>
+  </si>
+  <si>
+    <t>RU</t>
+  </si>
+  <si>
+    <t>WU</t>
+  </si>
+  <si>
+    <t>SR2</t>
+  </si>
+  <si>
+    <t>Part</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -218,8 +382,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="3"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF7030A0"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="3"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000099"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,8 +469,25 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -296,9 +530,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+  <cellStyleXfs count="26">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -315,31 +578,565 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="26">
+    <cellStyle name="20% - Accent1 2" xfId="25" xr:uid="{574CC6A7-43F9-4DD0-A080-86DE9DACDE7B}"/>
+    <cellStyle name="20% - Accent3 2" xfId="18" xr:uid="{E5274AB7-FE0C-42BA-966B-EDC596FC458D}"/>
     <cellStyle name="Bad" xfId="7" builtinId="27" hidden="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" hidden="1"/>
     <cellStyle name="Comment" xfId="16" xr:uid="{28F4129C-C7DD-498A-828E-8C4D762CC7A0}"/>
+    <cellStyle name="Comment 2" xfId="22" xr:uid="{8049095E-98D7-4C6A-A152-BDCDACDD8D6F}"/>
     <cellStyle name="Explanatory Text" xfId="14" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text 2" xfId="20" xr:uid="{F4E5F73E-9C5D-4ECF-A685-BFD2F1634DBE}"/>
     <cellStyle name="Good" xfId="6" builtinId="26" hidden="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 1 2" xfId="19" xr:uid="{EF747C85-A8A3-4693-A9C4-29B6BC90EAEE}"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 2 2" xfId="24" xr:uid="{454B2EFB-9C90-4C43-BF9E-E2AC58DD83E5}"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 3 2" xfId="23" xr:uid="{1F28CC29-8F9A-4338-8DD3-3CEEFCC4F9D5}"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Input 2" xfId="21" xr:uid="{08B27789-8764-44E0-8145-C03698894497}"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" hidden="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Normal 2" xfId="17" xr:uid="{E3F7A393-FC89-4953-BB13-9EF7D6982359}"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" hidden="1"/>
     <cellStyle name="Total" xfId="15" builtinId="25" hidden="1"/>
     <cellStyle name="Warning Text" xfId="13" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="39">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="double">
+          <color theme="6"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6"/>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+      <border diagonalDown="1">
+        <bottom style="double">
+          <color auto="1"/>
+        </bottom>
+        <diagonal style="double">
+          <color auto="1"/>
+        </diagonal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </bottom>
+        <horizontal style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEAEAEA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom/>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <top style="double">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="double">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
+  <tableStyles count="3" defaultTableStyle="Workout Style" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Biegert Standard" table="0" count="4" xr9:uid="{6717EBDB-3D97-4D30-B1E5-B03AA52F1420}">
+      <tableStyleElement type="headerRow" dxfId="38"/>
+      <tableStyleElement type="totalRow" dxfId="37"/>
+      <tableStyleElement type="firstColumn" dxfId="36"/>
+      <tableStyleElement type="firstRowStripe" dxfId="35"/>
+    </tableStyle>
+    <tableStyle name="Biegert Standard A" pivot="0" count="4" xr9:uid="{FC63C2DC-6FEA-4ABD-A934-4232587F4A71}">
+      <tableStyleElement type="headerRow" dxfId="34"/>
+      <tableStyleElement type="totalRow" dxfId="33"/>
+      <tableStyleElement type="firstColumn" dxfId="32"/>
+      <tableStyleElement type="firstRowStripe" dxfId="31"/>
+    </tableStyle>
+    <tableStyle name="Workout Style" pivot="0" count="7" xr9:uid="{570CB5D4-434C-491A-85D4-F6B08C33F6C3}">
+      <tableStyleElement type="wholeTable" dxfId="26"/>
+      <tableStyleElement type="headerRow" dxfId="25"/>
+      <tableStyleElement type="totalRow" dxfId="24"/>
+      <tableStyleElement type="firstColumn" dxfId="23"/>
+      <tableStyleElement type="lastColumn" dxfId="22"/>
+      <tableStyleElement type="firstRowStripe" dxfId="21"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="20"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -351,10 +1148,42 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{06D64AAF-801F-483B-829D-7089D1D26D3C}" name="_tW1" displayName="_tW1" ref="A1:W21" totalsRowShown="0" headerRowDxfId="30">
+  <autoFilter ref="A1:W21" xr:uid="{06D64AAF-801F-483B-829D-7089D1D26D3C}"/>
+  <tableColumns count="23">
+    <tableColumn id="1" xr3:uid="{29BF9500-CD46-47AD-9A96-1659607299E3}" name="Part" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{DBD6A2F4-25BF-4B3F-846B-65A13EC13A0F}" name="Exercise" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{2EA25E37-E8F5-4296-BD0C-821C57098731}" name="SS" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{5A4B101C-B1D7-4D51-81A0-9DD8EFD958CE}" name="RS" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{2367FDF5-ECE3-4ADD-8098-8F89495E4880}" name="WS" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{4D3CF3E9-E266-412A-BBA3-4E2BA1E60E22}" name="SM" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{FE7DBF9A-E3B9-4331-BBE4-1516825E665E}" name="RM" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{080C7007-E73B-4E05-856D-9A2967FBD025}" name="WM" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{1FD7A839-B091-4726-AB9B-C7861BF80C22}" name="ST" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{60712702-C73A-458F-92FE-F72407B9A6F6}" name="RT" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{EE1C1924-A0AA-47C6-880E-561A10BE72FA}" name="WT" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{AAADA156-A5CA-452D-B5FB-10BD00D0003F}" name="SW" dataDxfId="11"/>
+    <tableColumn id="13" xr3:uid="{672DA370-402E-4B40-85D7-AD9513D36B66}" name="RW" dataDxfId="10"/>
+    <tableColumn id="14" xr3:uid="{62739A32-0DCF-497A-B444-ADA42A4CE3E6}" name="WW" dataDxfId="9"/>
+    <tableColumn id="15" xr3:uid="{C79C317F-C384-44C8-BE2E-97BF7485A32F}" name="SR" dataDxfId="8"/>
+    <tableColumn id="16" xr3:uid="{D08F8672-09B7-4279-9CBB-4CBAA544851B}" name="RR" dataDxfId="7"/>
+    <tableColumn id="17" xr3:uid="{5A3D19F1-4BEC-4642-A6AE-D448D9E40D77}" name="WR" dataDxfId="6"/>
+    <tableColumn id="18" xr3:uid="{C7186DA1-EE3B-4427-9E91-B4C1CAB1CF24}" name="SR2" dataDxfId="5"/>
+    <tableColumn id="19" xr3:uid="{76B2045A-74F5-4EEE-A155-1E40CED43244}" name="RF" dataDxfId="4"/>
+    <tableColumn id="20" xr3:uid="{8C671214-3637-4E53-823C-B03772636DE1}" name="WF" dataDxfId="3"/>
+    <tableColumn id="21" xr3:uid="{B5C1A464-EDE4-4CE9-A4A5-27D21817053F}" name="SU" dataDxfId="2"/>
+    <tableColumn id="22" xr3:uid="{E5F1D46F-E2C5-4C03-8B58-90A54CDFDABC}" name="RU" dataDxfId="1"/>
+    <tableColumn id="23" xr3:uid="{AC0F6939-CACC-4C5B-8644-82C878B16CF7}" name="WU" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="Workout Style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Biegert-Standard">
   <a:themeElements>
-    <a:clrScheme name="Biegert-Complementary">
+    <a:clrScheme name="Spring_Pastels">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -368,28 +1197,28 @@
         <a:srgbClr val="DADADA"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="FF732B"/>
+        <a:srgbClr val="FD7F6F"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="B34A15"/>
+        <a:srgbClr val="7EB0D5"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="0C65B3"/>
+        <a:srgbClr val="B2E061"/>
       </a:accent3>
       <a:accent4>
         <a:srgbClr val="BD7EBE"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FFD82B"/>
+        <a:srgbClr val="FFB55A"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="B39204"/>
+        <a:srgbClr val="FFEE65"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0070C0"/>
+        <a:srgbClr val="BEB9DB"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="00B050"/>
+        <a:srgbClr val="FDCCE5"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Biegert-Standard">
@@ -579,8 +1408,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -688,4 +1517,716 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD944353-04A7-4C4C-A80D-ACC2549D41E0}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:W22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="23" width="8.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="2"/>
+    </row>
+    <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="2"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="2"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="2"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="2"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="2"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="2"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="2"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="2"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="2"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="2"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="2"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="2"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="2"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="2"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="2"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="2"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="2"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="2"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="7"/>
+      <c r="W21" s="2"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="61" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>